<commit_message>
this is my final commit
</commit_message>
<xml_diff>
--- a/output_excel_.xlsx
+++ b/output_excel_.xlsx
@@ -21,44 +21,44 @@
     <t>Doctor Description</t>
   </si>
   <si>
-    <t>Dr. Arati Sundar Rajan</t>
+    <t>Dr. Dinesh Shetty</t>
   </si>
   <si>
     <t>BDS
-Dentist
-28 Years Experience Overall</t>
-  </si>
-  <si>
-    <t>Dr. Ramya</t>
-  </si>
-  <si>
-    <t>BDS, MDS - Prosthodontics
-Prosthodontist, Dental Surgeon
-24 Years Experience Overall  (22 years as specialist)</t>
-  </si>
-  <si>
-    <t>Dr. Karthikeyan B.V</t>
-  </si>
-  <si>
-    <t>BDS, MDS - Periodontics
-Periodontist, Implantologist, Cosmetic/Aesthetic Dentist
-24 Years Experience Overall  (23 years as specialist)</t>
-  </si>
-  <si>
-    <t>Dr. Abhinav Diwan</t>
-  </si>
-  <si>
-    <t>BDS, MDS - Conservative Dentistry &amp; Endodontics
-Dentist, Endodontist, Implantologist
-25 Years Experience Overall  (23 years as specialist)</t>
-  </si>
-  <si>
-    <t>Dr. Pramod Kumar Pillai</t>
-  </si>
-  <si>
-    <t>BDS, Diploma in Implanthology
-Implantologist, Cosmetic/Aesthetic Dentist
-17 Years Experience Overall  (15 years as specialist)</t>
+Dentist, Dental Surgeon
+20 Years Experience Overall</t>
+  </si>
+  <si>
+    <t>Dr. Lokesh Babu</t>
+  </si>
+  <si>
+    <t>BDS, MDS - Oral &amp; Maxillofacial Surgery
+Dentist, Oral And MaxilloFacial Surgeon, Implantologist
+25 Years Experience Overall  (24 years as specialist)</t>
+  </si>
+  <si>
+    <t>Dr. Narayan Babu</t>
+  </si>
+  <si>
+    <t>BDS
+Dentist, Dental Surgeon, Cosmetic/Aesthetic Dentist
+16 Years Experience Overall</t>
+  </si>
+  <si>
+    <t>Dr. Divya Puranik</t>
+  </si>
+  <si>
+    <t>BDS, MDS - Orthodontics and Dentofacial Orthopaedics
+Orthodontist, Dentofacial Orthopedist
+15 Years Experience Overall  (9 years as specialist)</t>
+  </si>
+  <si>
+    <t>Dr. Nikhar Ravinder</t>
+  </si>
+  <si>
+    <t>BDS, MDS - Orthodontics and Dentofacial Orthopaedics
+Orthodontist, Dentist, Dental Surgeon, Dentofacial Orthopedist
+22 Years Experience Overall  (17 years as specialist)</t>
   </si>
   <si>
     <t>Popular Surgeries</t>

</xml_diff>